<commit_message>
update code and apply POM
</commit_message>
<xml_diff>
--- a/TestData/test.xlsx
+++ b/TestData/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nttr\PycharmProjects\RobotAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9A6A90-1DBC-4082-81A5-8002FED630D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5BDFC6-9746-4F9F-9058-2F1F8F99C909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{3233A5B0-2092-4258-B103-7A4373669FB7}"/>
   </bookViews>
@@ -133,7 +133,7 @@
     <t>def</t>
   </si>
   <si>
-    <t>trungtn9@yopmail.com</t>
+    <t>trungtn12@yopmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>